<commit_message>
Update web_scrap Update README
</commit_message>
<xml_diff>
--- a/data/hsr_paths_rarities_elements.xlsx
+++ b/data/hsr_paths_rarities_elements.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,12 +458,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>argenti</t>
+          <t>acheron</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Erudition</t>
+          <t>Nihility</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -473,41 +473,41 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Physical</t>
+          <t>Lightning</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>arlan</t>
+          <t>argenti</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Destruction</t>
+          <t>Erudition</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Lightning</t>
+          <t>Physical</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>asta</t>
+          <t>arlan</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Harmony</t>
+          <t>Destruction</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -517,41 +517,41 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Fire</t>
+          <t>Lightning</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>bailu</t>
+          <t>asta</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Abundance</t>
+          <t>Harmony</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Lightning</t>
+          <t>Fire</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>blade</t>
+          <t>aventurine</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Destruction</t>
+          <t>Preservation</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -561,19 +561,19 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Wind</t>
+          <t>Imaginary</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>bronya</t>
+          <t>bailu</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Harmony</t>
+          <t>Abundance</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -583,19 +583,19 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Wind</t>
+          <t>Lightning</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>clara</t>
+          <t>black-swan</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Destruction</t>
+          <t>Nihility</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -605,24 +605,24 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Physical</t>
+          <t>Wind</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>dan-heng</t>
+          <t>blade</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Hunt</t>
+          <t>Destruction</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -634,12 +634,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>imbibitor-lunae</t>
+          <t>bronya</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Destruction</t>
+          <t>Harmony</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -649,19 +649,19 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Imaginary</t>
+          <t>Wind</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>dr-ratio</t>
+          <t>clara</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Hunt</t>
+          <t>Destruction</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -671,41 +671,41 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Imaginary</t>
+          <t>Physical</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>fu-xuan</t>
+          <t>dan-heng</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Preservation</t>
+          <t>Hunt</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Quantum</t>
+          <t>Wind</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>gepard</t>
+          <t>imbibitor-lunae</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Preservation</t>
+          <t>Destruction</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -715,63 +715,63 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Ice</t>
+          <t>Imaginary</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>guinaifen</t>
+          <t>dr-ratio</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Nihility</t>
+          <t>Hunt</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Fire</t>
+          <t>Imaginary</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>hanya</t>
+          <t>fu-xuan</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Harmony</t>
+          <t>Preservation</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Physical</t>
+          <t>Quantum</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>herta</t>
+          <t>gallagher</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Erudition</t>
+          <t>Abundance</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -781,19 +781,19 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Ice</t>
+          <t>Fire</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>himeko</t>
+          <t>gepard</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Erudition</t>
+          <t>Preservation</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -803,19 +803,19 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Fire</t>
+          <t>Ice</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>hook</t>
+          <t>guinaifen</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Destruction</t>
+          <t>Nihility</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -832,29 +832,29 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>huohuo</t>
+          <t>hanya</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Abundance</t>
+          <t>Harmony</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Wind</t>
+          <t>Physical</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>jing-yuan</t>
+          <t>herta</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -864,24 +864,24 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Lightning</t>
+          <t>Ice</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>jingliu</t>
+          <t>himeko</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Destruction</t>
+          <t>Erudition</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -891,63 +891,63 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Ice</t>
+          <t>Fire</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>kafka</t>
+          <t>hook</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Nihility</t>
+          <t>Destruction</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Lightning</t>
+          <t>Fire</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>luka</t>
+          <t>huohuo</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Nihility</t>
+          <t>Abundance</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Physical</t>
+          <t>Wind</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>luocha</t>
+          <t>jing-yuan</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Abundance</t>
+          <t>Erudition</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -957,63 +957,63 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Imaginary</t>
+          <t>Lightning</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>lynx</t>
+          <t>jingliu</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Abundance</t>
+          <t>Destruction</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Quantum</t>
+          <t>Ice</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>march-7th</t>
+          <t>kafka</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Preservation</t>
+          <t>Nihility</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Ice</t>
+          <t>Lightning</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>natasha</t>
+          <t>luka</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Abundance</t>
+          <t>Nihility</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1030,34 +1030,34 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>pela</t>
+          <t>luocha</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Nihility</t>
+          <t>Abundance</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Ice</t>
+          <t>Imaginary</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>qingque</t>
+          <t>lynx</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Erudition</t>
+          <t>Abundance</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1074,17 +1074,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>ruan-mei</t>
+          <t>march-7th</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Harmony</t>
+          <t>Preservation</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1096,12 +1096,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>sampo</t>
+          <t>misha</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Nihility</t>
+          <t>Destruction</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1111,41 +1111,41 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Wind</t>
+          <t>Ice</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>seele</t>
+          <t>natasha</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Hunt</t>
+          <t>Abundance</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Quantum</t>
+          <t>Physical</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>serval</t>
+          <t>pela</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Erudition</t>
+          <t>Nihility</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1155,24 +1155,24 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Lightning</t>
+          <t>Ice</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>silver-wolf</t>
+          <t>qingque</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Nihility</t>
+          <t>Erudition</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1184,34 +1184,34 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>sushang</t>
+          <t>ruan-mei</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Hunt</t>
+          <t>Harmony</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Physical</t>
+          <t>Ice</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>tingyun</t>
+          <t>sampo</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Harmony</t>
+          <t>Nihility</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1221,14 +1221,14 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Lightning</t>
+          <t>Wind</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>topaz</t>
+          <t>seele</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1243,41 +1243,41 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Fire</t>
+          <t>Quantum</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>trailblazer-fire</t>
+          <t>serval</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Preservation</t>
+          <t>Erudition</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Fire</t>
+          <t>Lightning</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>trailblazer-physical</t>
+          <t>silver-wolf</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Destruction</t>
+          <t>Nihility</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1287,19 +1287,19 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Physical</t>
+          <t>Quantum</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>welt</t>
+          <t>sparkle</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Nihility</t>
+          <t>Harmony</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1309,19 +1309,19 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Imaginary</t>
+          <t>Quantum</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>xueyi</t>
+          <t>sushang</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Destruction</t>
+          <t>Hunt</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1331,49 +1331,181 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Quantum</t>
+          <t>Physical</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>yanqing</t>
+          <t>tingyun</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Hunt</t>
+          <t>Harmony</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Ice</t>
+          <t>Lightning</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>topaz</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Hunt</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Fire</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>trailblazer-fire</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Preservation</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Fire</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>trailblazer-physical</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Destruction</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Physical</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>welt</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Nihility</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Imaginary</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>xueyi</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Destruction</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Quantum</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>yanqing</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Hunt</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Ice</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
           <t>yukong</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B49" t="inlineStr">
         <is>
           <t>Harmony</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
         <is>
           <t>Imaginary</t>
         </is>

</xml_diff>